<commit_message>
Introduced my custom module, with proper formatting of the app messages. Updated my custom module
</commit_message>
<xml_diff>
--- a/story_templates.xlsx
+++ b/story_templates.xlsx
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added a story template
</commit_message>
<xml_diff>
--- a/story_templates.xlsx
+++ b/story_templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">NOUN; NOUN (PLURAL); NOUN; NOUN (PLURAL); PLACE; ADJECTIVE; NOUN </t>
   </si>
@@ -39,6 +39,23 @@
   </si>
   <si>
     <t>Story no.</t>
+  </si>
+  <si>
+    <t>Adjective;Adjective;Celebrity;Adjective;Time frame - plural;Noun - Plural;Adjective - Ends in ER;Verb - Base Form;Letter of Alphabet;Part of Body;Name that starts with S;Color;Color;Celebrity;Verb - Present ends in S;Noun;Color;Number;Number;Month;Number;Year;Month;Number;Year;Number;Day of the week</t>
+  </si>
+  <si>
+    <t>1. You know it's cold outside when you go outside, and it is {1}. 
+2. {2} had been {3} {4} before she was dead.
+3. Some {5} are {6} than others. 
+4. The future has yet to {7}. 
+5. The " {8} on Superman's {9} stands for {10}. 
+6. The sky is {11}, and the grass is {12}. 
+7. {13}'s last name is Obama. 
+8. Rain {14} from the {15}. 
+9. {16} is a color. 
+10. Take your age, subtract {17}, then add {18}. That is your age. 
+11. The 1950s lasted from {19} {20}, {21} - {22} {23}, {24}. 
+12. Friday the 13th occurs when the {25}th day of a month falls on a {26}.</t>
   </si>
 </sst>
 </file>
@@ -416,17 +433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="186.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -449,6 +466,14 @@
       </c>
       <c r="C2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>